<commit_message>
ultimas alterações para o extended
</commit_message>
<xml_diff>
--- a/AMPS2019/EXTENDED/comparisons.xlsx
+++ b/AMPS2019/EXTENDED/comparisons.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7590"/>
   </bookViews>
   <sheets>
-    <sheet name="II-B1" sheetId="3" r:id="rId1"/>
-    <sheet name="II-B2-FE" sheetId="1" r:id="rId2"/>
-    <sheet name="EPS comparison" sheetId="2" r:id="rId3"/>
+    <sheet name="FE" sheetId="4" r:id="rId1"/>
+    <sheet name="EPS comparison" sheetId="2" r:id="rId2"/>
+    <sheet name="II-B2-FE" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="88">
   <si>
     <t>FE_std_HE</t>
   </si>
@@ -78,21 +78,12 @@
     <t>Não sei ainda se teria alguma influência do ângulo phi_0 na estimação de frequencia.</t>
   </si>
   <si>
-    <t>kas = 10 graus</t>
-  </si>
-  <si>
-    <t>PATV</t>
-  </si>
-  <si>
     <t>FE</t>
   </si>
   <si>
     <t>FE_mean</t>
   </si>
   <si>
-    <t>FE_STD</t>
-  </si>
-  <si>
     <t>kas = -10</t>
   </si>
   <si>
@@ -136,21 +127,176 @@
   </si>
   <si>
     <t>kas</t>
+  </si>
+  <si>
+    <t>Table V</t>
+  </si>
+  <si>
+    <t>Table VI</t>
+  </si>
+  <si>
+    <t>SNR</t>
+  </si>
+  <si>
+    <t>case 2</t>
+  </si>
+  <si>
+    <t>case 3</t>
+  </si>
+  <si>
+    <t>km = 1.5e7;</t>
+  </si>
+  <si>
+    <t>kf = 1.1e7;</t>
+  </si>
+  <si>
+    <t>Table IV</t>
+  </si>
+  <si>
+    <t>case 1</t>
+  </si>
+  <si>
+    <t>mean [mHz/Hz]</t>
+  </si>
+  <si>
+    <t>std [mHz/Hz]</t>
+  </si>
+  <si>
+    <t>Case1</t>
+  </si>
+  <si>
+    <t>Case 3</t>
+  </si>
+  <si>
+    <t>phi0</t>
+  </si>
+  <si>
+    <t>lambda_theta_i = 1.;</t>
+  </si>
+  <si>
+    <t>lambda_a_i = 0.5;</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>muito alto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case 1 </t>
+  </si>
+  <si>
+    <t>Case 2</t>
+  </si>
+  <si>
+    <t>Talvez o kf e km pode ser otimizado</t>
+  </si>
+  <si>
+    <t>Ou seja melhor usar um valor absoluto</t>
+  </si>
+  <si>
+    <t>false pos</t>
+  </si>
+  <si>
+    <t>false neg</t>
+  </si>
+  <si>
+    <t>kf km relativos</t>
+  </si>
+  <si>
+    <t>kf km absolutos</t>
+  </si>
+  <si>
+    <t>fase pos</t>
+  </si>
+  <si>
+    <t>Falso positivo muito alto</t>
+  </si>
+  <si>
+    <t>razões possíveis:</t>
+  </si>
+  <si>
+    <t>identificando pelo detector de fase quando não devia?</t>
+  </si>
+  <si>
+    <t>não parece</t>
+  </si>
+  <si>
+    <t>modificação no cálculo do gradiente vs diff vs sinal u??</t>
+  </si>
+  <si>
+    <t>erro de 1?</t>
+  </si>
+  <si>
+    <t>diferença nenhuma</t>
+  </si>
+  <si>
+    <t>Pode ser do próprio PATV, que distorce o sinal</t>
+  </si>
+  <si>
+    <t>dmax min</t>
+  </si>
+  <si>
+    <t>median min</t>
+  </si>
+  <si>
+    <t>median max</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>mag</t>
+  </si>
+  <si>
+    <t>fase</t>
+  </si>
+  <si>
+    <t>th_a_i = 2.8e-3; th_fi = 4.8e-3;</t>
+  </si>
+  <si>
+    <t>limiares fixos</t>
+  </si>
+  <si>
+    <t>Os resultados são mais fáceis de otimizar com limiares fixos.</t>
+  </si>
+  <si>
+    <t>Como os sinais de detecção não estão corrompidos com ruído, a hipótese de gaussianidade fica muito fraca.</t>
+  </si>
+  <si>
+    <t>Isso faz com que a mediana do sinal fique muito variável, consequentemente o limiar determinado em função da mediana fica variável.</t>
+  </si>
+  <si>
+    <t>Os resultados ficam instáveis, oscilando entre falsos positivos e falsos negativos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case 2 </t>
+  </si>
+  <si>
+    <t>O desempenho melhora. Provavelmente é possível otimizar com os valores de limiares.</t>
+  </si>
+  <si>
+    <t>Outra otimização possível é a relação entre as razões no detector híbrido.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="8">
+  <numFmts count="10">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="173" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -202,22 +348,25 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,11 +545,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="330191280"/>
-        <c:axId val="331597520"/>
+        <c:axId val="251781112"/>
+        <c:axId val="251781504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="330191280"/>
+        <c:axId val="251781112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -457,12 +606,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331597520"/>
+        <c:crossAx val="251781504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="331597520"/>
+        <c:axId val="251781504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,7 +668,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330191280"/>
+        <c:crossAx val="251781112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -727,11 +876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="330192456"/>
-        <c:axId val="328569672"/>
+        <c:axId val="251782288"/>
+        <c:axId val="251782680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="330192456"/>
+        <c:axId val="251782288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -788,12 +937,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328569672"/>
+        <c:crossAx val="251782680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="328569672"/>
+        <c:axId val="251782680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,7 +999,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330192456"/>
+        <c:crossAx val="251782288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2363,17 +2512,1485 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8">
+        <v>60</v>
+      </c>
+      <c r="J8">
+        <v>50</v>
+      </c>
+      <c r="K8">
+        <v>40</v>
+      </c>
+      <c r="L8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8.6675147192722094E-6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8.4840411021506395E-6</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8.4644335825479192E-6</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4.6525502333783302E-6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="4">
+        <f>C9*1000</f>
+        <v>8.6675147192722089E-3</v>
+      </c>
+      <c r="J9" s="4">
+        <f t="shared" ref="J9:J10" si="0">D9*1000</f>
+        <v>8.4840411021506398E-3</v>
+      </c>
+      <c r="K9" s="4">
+        <f t="shared" ref="K9:K10" si="1">E9*1000</f>
+        <v>8.46443358254792E-3</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" ref="L9:L10" si="2">F9*1000</f>
+        <v>4.6525502333783298E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4.1250610612548203E-6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1.31051588655984E-5</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4.1417158658526197E-5</v>
+      </c>
+      <c r="F10">
+        <v>1.3148393612150299E-4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="4">
+        <f>C10*1000</f>
+        <v>4.12506106125482E-3</v>
+      </c>
+      <c r="J10" s="4">
+        <f t="shared" si="0"/>
+        <v>1.3105158865598399E-2</v>
+      </c>
+      <c r="K10" s="4">
+        <f t="shared" si="1"/>
+        <v>4.1417158658526194E-2</v>
+      </c>
+      <c r="L10" s="4">
+        <f t="shared" si="2"/>
+        <v>0.131483936121503</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13">
+        <v>60</v>
+      </c>
+      <c r="D13">
+        <v>50</v>
+      </c>
+      <c r="E13">
+        <v>40</v>
+      </c>
+      <c r="F13">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13">
+        <v>60</v>
+      </c>
+      <c r="J13">
+        <v>50</v>
+      </c>
+      <c r="K13">
+        <v>40</v>
+      </c>
+      <c r="L13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1.3274392824296701E-3</v>
+      </c>
+      <c r="D14">
+        <v>1.31627671255559E-3</v>
+      </c>
+      <c r="E14">
+        <v>1.2887847598532999E-3</v>
+      </c>
+      <c r="F14">
+        <v>1.25482371591755E-3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="13">
+        <f>C14*1000</f>
+        <v>1.3274392824296701</v>
+      </c>
+      <c r="J14" s="13">
+        <f t="shared" ref="J14:L15" si="3">D14*1000</f>
+        <v>1.3162767125555899</v>
+      </c>
+      <c r="K14" s="13">
+        <f t="shared" si="3"/>
+        <v>1.2887847598533</v>
+      </c>
+      <c r="L14" s="13">
+        <f t="shared" si="3"/>
+        <v>1.2548237159175499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1">
+        <v>8.5110464310568807E-6</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2.64340316087002E-5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>8.4209716461973699E-5</v>
+      </c>
+      <c r="F15">
+        <v>2.6649080307221998E-4</v>
+      </c>
+      <c r="H15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="4">
+        <f>C15*1000</f>
+        <v>8.5110464310568807E-3</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="3"/>
+        <v>2.6434031608700198E-2</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" si="3"/>
+        <v>8.4209716461973699E-2</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" si="3"/>
+        <v>0.26649080307221995</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18">
+        <v>60</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+      <c r="E18">
+        <v>40</v>
+      </c>
+      <c r="F18">
+        <v>30</v>
+      </c>
+      <c r="H18" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18">
+        <v>60</v>
+      </c>
+      <c r="J18">
+        <v>50</v>
+      </c>
+      <c r="K18">
+        <v>40</v>
+      </c>
+      <c r="L18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>1.1817832356779501E-3</v>
+      </c>
+      <c r="D19">
+        <v>1.1798809688730999E-3</v>
+      </c>
+      <c r="E19">
+        <v>1.1730693809531899E-3</v>
+      </c>
+      <c r="F19">
+        <v>1.1684859453060001E-3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="13">
+        <f>C19*1000</f>
+        <v>1.1817832356779501</v>
+      </c>
+      <c r="J19" s="13">
+        <f t="shared" ref="J19:J20" si="4">D19*1000</f>
+        <v>1.1798809688731</v>
+      </c>
+      <c r="K19" s="13">
+        <f t="shared" ref="K19:K20" si="5">E19*1000</f>
+        <v>1.1730693809531898</v>
+      </c>
+      <c r="L19" s="13">
+        <f t="shared" ref="L19:L20" si="6">F19*1000</f>
+        <v>1.1684859453060001</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1">
+        <v>9.1970074191314105E-6</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2.8832854333037099E-5</v>
+      </c>
+      <c r="E20" s="1">
+        <v>9.0535506127008901E-5</v>
+      </c>
+      <c r="F20">
+        <v>2.9116843944998499E-4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" s="4">
+        <f>C20*1000</f>
+        <v>9.1970074191314102E-3</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="4"/>
+        <v>2.8832854333037099E-2</v>
+      </c>
+      <c r="K20" s="4">
+        <f t="shared" si="5"/>
+        <v>9.0535506127008905E-2</v>
+      </c>
+      <c r="L20" s="4">
+        <f t="shared" si="6"/>
+        <v>0.29116843944998499</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:Z69"/>
+  <sheetViews>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="W5" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O6" s="1"/>
+      <c r="Q6" t="s">
+        <v>64</v>
+      </c>
+      <c r="V6" t="s">
+        <v>50</v>
+      </c>
+      <c r="W6">
+        <v>60</v>
+      </c>
+      <c r="X6">
+        <v>50</v>
+      </c>
+      <c r="Y6">
+        <v>40</v>
+      </c>
+      <c r="Z6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="H8">
+        <v>40</v>
+      </c>
+      <c r="J8">
+        <v>40</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="Q8" t="s">
+        <v>65</v>
+      </c>
+      <c r="V8">
+        <f>V7+15</f>
+        <v>15</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>42.9</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>42.9</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="15">
+        <v>0</v>
+      </c>
+      <c r="O9" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>66</v>
+      </c>
+      <c r="V9">
+        <f>V8+15</f>
+        <v>30</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>A9+15</f>
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>62.3</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>62.3</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="15">
+        <v>0</v>
+      </c>
+      <c r="O10" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>67</v>
+      </c>
+      <c r="V10">
+        <f>V9+15</f>
+        <v>45</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>1.4</v>
+      </c>
+      <c r="Z10">
+        <v>39.200000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>A10+15</f>
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>82.2</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="H11">
+        <v>0.4</v>
+      </c>
+      <c r="J11">
+        <v>81.8</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="O11" s="15">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <f>V10+15</f>
+        <v>60</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>2.8</v>
+      </c>
+      <c r="Z11">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>A11+15</f>
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <v>94.9</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="H12">
+        <v>63.7</v>
+      </c>
+      <c r="J12">
+        <v>31.2</v>
+      </c>
+      <c r="M12">
+        <v>1.37</v>
+      </c>
+      <c r="N12" s="15">
+        <v>1.25</v>
+      </c>
+      <c r="O12" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>68</v>
+      </c>
+      <c r="V12">
+        <f>V11+15</f>
+        <v>75</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>8.4</v>
+      </c>
+      <c r="Z12">
+        <v>53.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>A12+15</f>
+        <v>60</v>
+      </c>
+      <c r="D13">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="M13">
+        <v>2.83</v>
+      </c>
+      <c r="N13" s="15">
+        <v>2.71</v>
+      </c>
+      <c r="O13" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>69</v>
+      </c>
+      <c r="V13">
+        <f>V12+15</f>
+        <v>90</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0.9</v>
+      </c>
+      <c r="Y13">
+        <v>25.8</v>
+      </c>
+      <c r="Z13">
+        <v>53.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>A13+15</f>
+        <v>75</v>
+      </c>
+      <c r="D14">
+        <v>42.1</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="H14">
+        <v>5.3</v>
+      </c>
+      <c r="J14">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="M14">
+        <v>8.44</v>
+      </c>
+      <c r="N14" s="15">
+        <v>8.08</v>
+      </c>
+      <c r="O14" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>A14+15</f>
+        <v>90</v>
+      </c>
+      <c r="D15">
+        <v>37.9</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="H15">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="J15">
+        <v>20.3</v>
+      </c>
+      <c r="M15">
+        <v>23.31</v>
+      </c>
+      <c r="N15" s="15">
+        <v>23.67</v>
+      </c>
+      <c r="O15" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Q16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18">
+        <v>60</v>
+      </c>
+      <c r="C18">
+        <v>50</v>
+      </c>
+      <c r="D18">
+        <v>40</v>
+      </c>
+      <c r="E18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f>A19+15</f>
+        <v>15</v>
+      </c>
+      <c r="E20" s="14"/>
+      <c r="P20" t="s">
+        <v>77</v>
+      </c>
+      <c r="S20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f>A20+15</f>
+        <v>30</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="O21" t="s">
+        <v>72</v>
+      </c>
+      <c r="P21">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="R21" t="s">
+        <v>72</v>
+      </c>
+      <c r="S21" s="1">
+        <v>9.7000000000000003E-3</v>
+      </c>
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>A21+15</f>
+        <v>45</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="O22" t="s">
+        <v>73</v>
+      </c>
+      <c r="P22" s="1">
+        <v>1.0699999999999999E-11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>A22+15</f>
+        <v>60</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="O23" t="s">
+        <v>74</v>
+      </c>
+      <c r="P23" s="1">
+        <v>1.2400000000000001E-9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>A23+15</f>
+        <v>75</v>
+      </c>
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>A24+15</f>
+        <v>90</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="O25" t="s">
+        <v>75</v>
+      </c>
+      <c r="P25">
+        <f>P21/2</f>
+        <v>2.8500000000000001E-3</v>
+      </c>
+      <c r="R25" t="s">
+        <v>75</v>
+      </c>
+      <c r="S25">
+        <f>S21/2</f>
+        <v>4.8500000000000001E-3</v>
+      </c>
+      <c r="T25">
+        <f>S25/P25</f>
+        <v>1.7017543859649122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="O26" t="s">
+        <v>76</v>
+      </c>
+      <c r="P26" s="1">
+        <f>P25/P22</f>
+        <v>266355140.1869159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27">
+        <v>60</v>
+      </c>
+      <c r="C27">
+        <v>50</v>
+      </c>
+      <c r="D27">
+        <v>40</v>
+      </c>
+      <c r="E27">
+        <v>30</v>
+      </c>
+      <c r="O27" t="s">
+        <v>76</v>
+      </c>
+      <c r="P27" s="1">
+        <f>P25/P23</f>
+        <v>2298387.0967741935</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="G28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f>A28+15</f>
+        <v>15</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="G29" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f>A29+15</f>
+        <v>30</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="I30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f>A30+15</f>
+        <v>45</v>
+      </c>
+      <c r="E31" s="14"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f>A31+15</f>
+        <v>60</v>
+      </c>
+      <c r="E32" s="14"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f>A32+15</f>
+        <v>75</v>
+      </c>
+      <c r="E33" s="14"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f>A33+15</f>
+        <v>90</v>
+      </c>
+      <c r="E34" s="14"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40">
+        <v>60</v>
+      </c>
+      <c r="C40">
+        <v>50</v>
+      </c>
+      <c r="D40">
+        <v>40</v>
+      </c>
+      <c r="E40">
+        <v>30</v>
+      </c>
+      <c r="H40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41" s="14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f>A41+15</f>
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="H42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f>A42+15</f>
+        <v>30</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" s="14">
+        <v>4</v>
+      </c>
+      <c r="H43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f>A43+15</f>
+        <v>45</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44" s="14">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f>A44+15</f>
+        <v>60</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0.9</v>
+      </c>
+      <c r="E45" s="14">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f>A45+15</f>
+        <v>75</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E46" s="14">
+        <v>45</v>
+      </c>
+      <c r="H46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f>A46+15</f>
+        <v>90</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D47">
+        <v>25.6</v>
+      </c>
+      <c r="E47" s="14">
+        <v>55.5</v>
+      </c>
+      <c r="H47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>60</v>
+      </c>
+      <c r="C51">
+        <v>50</v>
+      </c>
+      <c r="D51">
+        <v>40</v>
+      </c>
+      <c r="E51">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>6.7</v>
+      </c>
+      <c r="E52" s="14">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f>A52+15</f>
+        <v>15</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0.5</v>
+      </c>
+      <c r="E53" s="14">
+        <v>27.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f>A53+15</f>
+        <v>30</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" s="14">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f>A54+15</f>
+        <v>45</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55" s="14">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f>A55+15</f>
+        <v>60</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f>A56+15</f>
+        <v>75</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f>A57+15</f>
+        <v>90</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>50</v>
+      </c>
+      <c r="B62">
+        <v>60</v>
+      </c>
+      <c r="C62">
+        <v>50</v>
+      </c>
+      <c r="D62">
+        <v>40</v>
+      </c>
+      <c r="E62">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63" s="14">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f>A63+15</f>
+        <v>15</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64" s="14">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f>A64+15</f>
+        <v>30</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65" s="14">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f>A65+15</f>
+        <v>45</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0.1</v>
+      </c>
+      <c r="E66" s="14">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f>A66+15</f>
+        <v>60</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67" s="14">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f>A67+15</f>
+        <v>75</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68" s="14">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f>A68+15</f>
+        <v>90</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69" s="14">
+        <v>4.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M55"/>
   <sheetViews>
@@ -2784,7 +4401,7 @@
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G30" s="6"/>
       <c r="J30" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2841,12 +4458,12 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B38">
         <v>60</v>
@@ -2863,7 +4480,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B39" s="4">
         <v>-1.8985172077897101E-3</v>
@@ -2894,7 +4511,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B42" s="4">
         <v>-1.14411466143884E-3</v>
@@ -2909,7 +4526,7 @@
         <v>-1.13916299235699E-3</v>
       </c>
       <c r="G42" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -2926,17 +4543,17 @@
         <v>4.9632987227239103E-4</v>
       </c>
       <c r="G43" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B45" s="4">
         <v>-5.2528405083098698E-4</v>
@@ -2951,7 +4568,7 @@
         <v>-5.3310761789805098E-4</v>
       </c>
       <c r="H45" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2968,16 +4585,16 @@
         <v>5.5323714320546597E-4</v>
       </c>
       <c r="H46" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I46" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J46" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L46" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2996,7 +4613,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B48" s="3">
         <v>6.3790293082863702E-6</v>
@@ -3068,7 +4685,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B51" s="4">
         <v>5.6858121833954802E-4</v>
@@ -3140,7 +4757,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B54" s="4">
         <v>9.2585088157849595E-4</v>
@@ -3199,301 +4816,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6:Q12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>2.2125025294899799E-3</v>
-      </c>
-      <c r="J6">
-        <v>2.1934373724922002E-3</v>
-      </c>
-      <c r="K6">
-        <v>2.1474178095515E-3</v>
-      </c>
-      <c r="L6">
-        <v>2.0856218540179299E-3</v>
-      </c>
-      <c r="N6" s="1">
-        <v>1.41678800463697E-5</v>
-      </c>
-      <c r="O6" s="1">
-        <v>4.4287369757191802E-5</v>
-      </c>
-      <c r="P6">
-        <v>1.3885142683918799E-4</v>
-      </c>
-      <c r="Q6">
-        <v>4.4423225817998198E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>2.2125080234570399E-3</v>
-      </c>
-      <c r="J7">
-        <v>2.1934044651903801E-3</v>
-      </c>
-      <c r="K7">
-        <v>2.14685310520821E-3</v>
-      </c>
-      <c r="L7">
-        <v>2.0904798686203598E-3</v>
-      </c>
-      <c r="N7" s="1">
-        <v>1.4015834874032001E-5</v>
-      </c>
-      <c r="O7" s="1">
-        <v>4.4013014169035201E-5</v>
-      </c>
-      <c r="P7">
-        <v>1.3801978129326101E-4</v>
-      </c>
-      <c r="Q7">
-        <v>4.4499719130213498E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>2.2126785776689401E-3</v>
-      </c>
-      <c r="J8">
-        <v>2.1938362810644402E-3</v>
-      </c>
-      <c r="K8">
-        <v>2.1476906784019399E-3</v>
-      </c>
-      <c r="L8">
-        <v>2.0985714115193599E-3</v>
-      </c>
-      <c r="N8" s="1">
-        <v>1.3911189943835299E-5</v>
-      </c>
-      <c r="O8" s="1">
-        <v>4.33403373487918E-5</v>
-      </c>
-      <c r="P8">
-        <v>1.41234598098615E-4</v>
-      </c>
-      <c r="Q8">
-        <v>4.4516382592519498E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>2.2126228379139999E-3</v>
-      </c>
-      <c r="J9">
-        <v>2.19412870818221E-3</v>
-      </c>
-      <c r="K9">
-        <v>2.1468735845302702E-3</v>
-      </c>
-      <c r="L9">
-        <v>2.0861328745990998E-3</v>
-      </c>
-      <c r="N9" s="1">
-        <v>1.3876364257070799E-5</v>
-      </c>
-      <c r="O9" s="1">
-        <v>4.4350995418859902E-5</v>
-      </c>
-      <c r="P9">
-        <v>1.3934868589947499E-4</v>
-      </c>
-      <c r="Q9">
-        <v>4.4485398939897902E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>2.21266650523551E-3</v>
-      </c>
-      <c r="J10">
-        <v>2.1936388216520801E-3</v>
-      </c>
-      <c r="K10">
-        <v>2.1454369035184802E-3</v>
-      </c>
-      <c r="L10">
-        <v>2.0850583393036302E-3</v>
-      </c>
-      <c r="N10" s="1">
-        <v>1.41239313928432E-5</v>
-      </c>
-      <c r="O10" s="1">
-        <v>4.4078893475494999E-5</v>
-      </c>
-      <c r="P10">
-        <v>1.3920430179989199E-4</v>
-      </c>
-      <c r="Q10">
-        <v>4.44639123696454E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>2.21281360671976E-3</v>
-      </c>
-      <c r="J11">
-        <v>2.1933756950027099E-3</v>
-      </c>
-      <c r="K11">
-        <v>2.1478273526456199E-3</v>
-      </c>
-      <c r="L11">
-        <v>2.0923955193802401E-3</v>
-      </c>
-      <c r="N11" s="1">
-        <v>1.3986991323090799E-5</v>
-      </c>
-      <c r="O11" s="1">
-        <v>4.4016786620159702E-5</v>
-      </c>
-      <c r="P11">
-        <v>1.3900204502960501E-4</v>
-      </c>
-      <c r="Q11">
-        <v>4.4696574684306001E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>2.21277236853938E-3</v>
-      </c>
-      <c r="J12">
-        <v>2.1940784801676898E-3</v>
-      </c>
-      <c r="K12">
-        <v>2.14621374177348E-3</v>
-      </c>
-      <c r="L12">
-        <v>2.0917072270902801E-3</v>
-      </c>
-      <c r="N12" s="1">
-        <v>1.40967890252059E-5</v>
-      </c>
-      <c r="O12" s="1">
-        <v>4.3894539640871401E-5</v>
-      </c>
-      <c r="P12">
-        <v>1.3902056635483001E-4</v>
-      </c>
-      <c r="Q12">
-        <v>4.4420610056820198E-4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
aumentei a freq chaveamento
</commit_message>
<xml_diff>
--- a/AMPS2019/EXTENDED/comparisons.xlsx
+++ b/AMPS2019/EXTENDED/comparisons.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="224">
   <si>
     <t>FE_std_HE</t>
   </si>
@@ -622,9 +622,6 @@
     <t>phi_0_est</t>
   </si>
   <si>
-    <t>FE_std</t>
-  </si>
-  <si>
     <t>correção @ 60dB</t>
   </si>
   <si>
@@ -666,6 +663,48 @@
   <si>
     <t>FE_mean [Hz/Hz]</t>
   </si>
+  <si>
+    <t>Aproximando a freq pela média de gradient(theta)</t>
+  </si>
+  <si>
+    <t>&lt;&lt; faz sentido aplicar o PATV?</t>
+  </si>
+  <si>
+    <t>&lt;&lt; lambda não é capaz de realizar uma compensação suficiente</t>
+  </si>
+  <si>
+    <t>pois continua fortemente dependente do ruído e da fase inicial</t>
+  </si>
+  <si>
+    <t>FE_std [Hz/Hz]</t>
+  </si>
+  <si>
+    <t>FE[Hz/Hz]</t>
+  </si>
+  <si>
+    <t>std FE [Hz/Hz]</t>
+  </si>
+  <si>
+    <t>O erro sistemático é menor do que o estimador baseado na mediana de f_i, mas o desvio padrão é maior.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">erro </t>
+  </si>
+  <si>
+    <t>f0</t>
+  </si>
+  <si>
+    <t>ferr</t>
+  </si>
+  <si>
+    <t>aumentando a freq chaveamento melhora !!!</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>Hz/Hz</t>
+  </si>
 </sst>
 </file>
 
@@ -684,8 +723,8 @@
     <numFmt numFmtId="172" formatCode="#,##0.0"/>
     <numFmt numFmtId="173" formatCode="0.00000000"/>
     <numFmt numFmtId="174" formatCode="0.000000E+00"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;????_-;_-@_-"/>
+    <numFmt numFmtId="175" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;????_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -848,7 +887,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -890,11 +929,14 @@
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1077,11 +1119,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="227675664"/>
-        <c:axId val="190750128"/>
+        <c:axId val="121719400"/>
+        <c:axId val="157056696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="227675664"/>
+        <c:axId val="121719400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1138,12 +1180,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190750128"/>
+        <c:crossAx val="157056696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="190750128"/>
+        <c:axId val="157056696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1200,7 +1242,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227675664"/>
+        <c:crossAx val="121719400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1412,11 +1454,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="227682168"/>
-        <c:axId val="227682552"/>
+        <c:axId val="157451176"/>
+        <c:axId val="121717832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="227682168"/>
+        <c:axId val="157451176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,12 +1515,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227682552"/>
+        <c:crossAx val="121717832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="227682552"/>
+        <c:axId val="121717832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1535,7 +1577,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227682168"/>
+        <c:crossAx val="157451176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1745,7 +1787,7 @@
             <c:numRef>
               <c:f>'FE-causas'!$D$10:$D$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_-* #,##0.000000_-;\-* #,##0.000000_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2.9833449605428902E-3</c:v>
@@ -1753,19 +1795,19 @@
                 <c:pt idx="1">
                   <c:v>2.96427106058507E-3</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0.00E+00">
+                <c:pt idx="2">
                   <c:v>2.9658976107004298E-3</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.00E+00">
+                <c:pt idx="3">
                   <c:v>3.0599198172934802E-3</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0.00E+00">
+                <c:pt idx="4">
                   <c:v>3.2328797267836898E-3</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00E+00">
+                <c:pt idx="5">
                   <c:v>3.3847162508287899E-3</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="0.00E+00">
+                <c:pt idx="6">
                   <c:v>3.4266982720288701E-3</c:v>
                 </c:pt>
               </c:numCache>
@@ -1781,11 +1823,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="190075872"/>
-        <c:axId val="190076264"/>
+        <c:axId val="221707704"/>
+        <c:axId val="156102744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="190075872"/>
+        <c:axId val="221707704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1842,12 +1884,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190076264"/>
+        <c:crossAx val="156102744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="190076264"/>
+        <c:axId val="156102744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1867,7 +1909,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1904,7 +1946,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190075872"/>
+        <c:crossAx val="221707704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3641,7 +3683,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3677,7 +3719,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5638,19 +5680,27 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z68"/>
+  <dimension ref="A1:Z94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -5678,7 +5728,7 @@
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
       <c r="W4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
@@ -5767,7 +5817,7 @@
         <v>3.1453896712518889E-3</v>
       </c>
       <c r="O8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P8" t="s">
         <v>153</v>
@@ -5778,7 +5828,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E9" s="22">
         <v>50</v>
@@ -5796,13 +5846,13 @@
         <v>195</v>
       </c>
       <c r="P9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="R9" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
@@ -5812,20 +5862,20 @@
       <c r="C10" s="22">
         <v>0</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="42">
         <v>2.9833449605428902E-3</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="43">
         <v>2.9830740291139001E-3</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="43">
         <v>2.9856236988032498E-3</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="43">
         <v>2.9650229597465998E-3</v>
       </c>
       <c r="I10" s="37">
-        <f t="shared" ref="I10:I16" si="1">(D10-$I$8)*1000000</f>
+        <f>(D10-$I$8)*1000000</f>
         <v>-162.04471070899868</v>
       </c>
       <c r="N10" s="22">
@@ -5851,23 +5901,23 @@
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C11" s="22">
-        <f t="shared" ref="C11:C16" si="2">C10+15</f>
+        <f t="shared" ref="C11:C16" si="1">C10+15</f>
         <v>15</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="43">
         <v>2.96427106058507E-3</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="43">
         <v>2.9636644484178402E-3</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="43">
         <v>2.9696511399392501E-3</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="43">
         <v>2.9573867417583399E-3</v>
       </c>
       <c r="I11" s="37">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I10:I16" si="2">(D11-$I$8)*1000000</f>
         <v>-181.11861066681885</v>
       </c>
       <c r="N11" s="22">
@@ -5878,7 +5928,7 @@
         <v>14.02</v>
       </c>
       <c r="P11" s="38">
-        <f t="shared" ref="P10:P16" si="4">D11</f>
+        <f t="shared" ref="P11:P16" si="4">D11</f>
         <v>2.96427106058507E-3</v>
       </c>
       <c r="Q11" s="1">
@@ -5893,23 +5943,23 @@
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C12" s="22">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="D12" s="43">
+        <v>2.9658976107004298E-3</v>
+      </c>
+      <c r="E12" s="43">
+        <v>2.9665716523075902E-3</v>
+      </c>
+      <c r="F12" s="43">
+        <v>2.9687694857133099E-3</v>
+      </c>
+      <c r="G12" s="43">
+        <v>2.9623773286500199E-3</v>
+      </c>
+      <c r="I12" s="37">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2.9658976107004298E-3</v>
-      </c>
-      <c r="E12" s="1">
-        <v>2.9665716523075902E-3</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2.9687694857133099E-3</v>
-      </c>
-      <c r="G12">
-        <v>2.9623773286500199E-3</v>
-      </c>
-      <c r="I12" s="37">
-        <f t="shared" si="1"/>
         <v>-179.4920605514591</v>
       </c>
       <c r="N12" s="22">
@@ -5935,23 +5985,23 @@
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C13" s="22">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="D13" s="43">
+        <v>3.0599198172934802E-3</v>
+      </c>
+      <c r="E13" s="43">
+        <v>3.0605195500214202E-3</v>
+      </c>
+      <c r="F13" s="43">
+        <v>3.0603759658641401E-3</v>
+      </c>
+      <c r="G13" s="43">
+        <v>3.0565053562884299E-3</v>
+      </c>
+      <c r="I13" s="37">
         <f t="shared" si="2"/>
-        <v>45</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3.0599198172934802E-3</v>
-      </c>
-      <c r="E13" s="1">
-        <v>3.0605195500214202E-3</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3.0603759658641401E-3</v>
-      </c>
-      <c r="G13">
-        <v>3.0565053562884299E-3</v>
-      </c>
-      <c r="I13" s="37">
-        <f t="shared" si="1"/>
         <v>-85.469853958408663</v>
       </c>
       <c r="N13" s="22">
@@ -5977,23 +6027,23 @@
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C14" s="22">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="D14" s="43">
+        <v>3.2328797267836898E-3</v>
+      </c>
+      <c r="E14" s="43">
+        <v>3.2335752915547502E-3</v>
+      </c>
+      <c r="F14" s="43">
+        <v>3.2437878909207401E-3</v>
+      </c>
+      <c r="G14" s="43">
+        <v>3.23046504489914E-3</v>
+      </c>
+      <c r="I14" s="37">
         <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="D14" s="1">
-        <v>3.2328797267836898E-3</v>
-      </c>
-      <c r="E14" s="1">
-        <v>3.2335752915547502E-3</v>
-      </c>
-      <c r="F14" s="1">
-        <v>3.2437878909207401E-3</v>
-      </c>
-      <c r="G14">
-        <v>3.23046504489914E-3</v>
-      </c>
-      <c r="I14" s="37">
-        <f t="shared" si="1"/>
         <v>87.490055531800905</v>
       </c>
       <c r="N14" s="22">
@@ -6019,23 +6069,23 @@
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C15" s="22">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="D15" s="43">
+        <v>3.3847162508287899E-3</v>
+      </c>
+      <c r="E15" s="43">
+        <v>3.3858834611352E-3</v>
+      </c>
+      <c r="F15" s="43">
+        <v>3.3877276842113001E-3</v>
+      </c>
+      <c r="G15" s="43">
+        <v>3.3773683272386099E-3</v>
+      </c>
+      <c r="I15" s="37">
         <f t="shared" si="2"/>
-        <v>75</v>
-      </c>
-      <c r="D15" s="1">
-        <v>3.3847162508287899E-3</v>
-      </c>
-      <c r="E15" s="1">
-        <v>3.3858834611352E-3</v>
-      </c>
-      <c r="F15" s="1">
-        <v>3.3877276842113001E-3</v>
-      </c>
-      <c r="G15">
-        <v>3.3773683272386099E-3</v>
-      </c>
-      <c r="I15" s="37">
-        <f t="shared" si="1"/>
         <v>239.326579576901</v>
       </c>
       <c r="N15" s="22">
@@ -6061,23 +6111,23 @@
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C16" s="22">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="D16" s="43">
+        <v>3.4266982720288701E-3</v>
+      </c>
+      <c r="E16" s="43">
+        <v>3.4260835842907099E-3</v>
+      </c>
+      <c r="F16" s="43">
+        <v>3.4286377413187E-3</v>
+      </c>
+      <c r="G16" s="43">
+        <v>3.4252148969755401E-3</v>
+      </c>
+      <c r="I16" s="37">
         <f t="shared" si="2"/>
-        <v>90</v>
-      </c>
-      <c r="D16" s="1">
-        <v>3.4266982720288701E-3</v>
-      </c>
-      <c r="E16" s="1">
-        <v>3.4260835842907099E-3</v>
-      </c>
-      <c r="F16" s="1">
-        <v>3.4286377413187E-3</v>
-      </c>
-      <c r="G16">
-        <v>3.4252148969755401E-3</v>
-      </c>
-      <c r="I16" s="37">
-        <f t="shared" si="1"/>
         <v>281.30860077698117</v>
       </c>
       <c r="N16" s="22">
@@ -6111,7 +6161,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="O18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -7182,18 +7232,18 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B57">
         <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -7201,31 +7251,31 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B60" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C60" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="B61" s="40">
+      <c r="B61" s="39">
         <v>2.7E-2</v>
       </c>
-      <c r="C61" s="41">
+      <c r="C61" s="40">
         <f>1000000*B61/60</f>
         <v>450</v>
       </c>
@@ -7234,10 +7284,10 @@
       <c r="A62" s="1">
         <v>1E-4</v>
       </c>
-      <c r="B62" s="40">
+      <c r="B62" s="39">
         <v>-7.4000000000000003E-3</v>
       </c>
-      <c r="C62" s="41">
+      <c r="C62" s="40">
         <f t="shared" ref="C62:C68" si="11">1000000*B62/60</f>
         <v>-123.33333333333333</v>
       </c>
@@ -7246,10 +7296,10 @@
       <c r="A63" s="1">
         <v>1E-3</v>
       </c>
-      <c r="B63" s="40">
+      <c r="B63" s="39">
         <v>-8.2000000000000007E-3</v>
       </c>
-      <c r="C63" s="41">
+      <c r="C63" s="40">
         <f t="shared" si="11"/>
         <v>-136.66666666666666</v>
       </c>
@@ -7258,60 +7308,405 @@
       <c r="A64" s="1">
         <v>0.01</v>
       </c>
-      <c r="B64" s="40">
+      <c r="B64" s="39">
         <v>-1.2E-2</v>
       </c>
-      <c r="C64" s="41">
+      <c r="C64" s="40">
         <f t="shared" si="11"/>
         <v>-200</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>0.1</v>
       </c>
-      <c r="B65" s="40">
+      <c r="B65" s="39">
         <v>-1.1999999999999999E-3</v>
       </c>
-      <c r="C65" s="41">
+      <c r="C65" s="40">
         <f t="shared" si="11"/>
         <v>-20</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>0.5</v>
       </c>
-      <c r="B66" s="40">
+      <c r="B66" s="39">
         <v>-2.3340000000000001E-4</v>
       </c>
-      <c r="C66" s="41">
+      <c r="C66" s="40">
         <f t="shared" si="11"/>
         <v>-3.89</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>1</v>
       </c>
-      <c r="B67" s="40">
+      <c r="B67" s="39">
         <v>3.9E-2</v>
       </c>
-      <c r="C67" s="41">
+      <c r="C67" s="40">
         <f t="shared" si="11"/>
         <v>650</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>2.5</v>
       </c>
-      <c r="B68" s="40">
+      <c r="B68" s="39">
         <v>0.17899999999999999</v>
       </c>
-      <c r="C68" s="41">
+      <c r="C68" s="40">
         <f t="shared" si="11"/>
         <v>2983.3333333333335</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>210</v>
+      </c>
+      <c r="G72" s="36"/>
+      <c r="K72" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>215</v>
+      </c>
+      <c r="B73" s="22">
+        <v>60</v>
+      </c>
+      <c r="C73" s="22">
+        <v>50</v>
+      </c>
+      <c r="D73" s="22">
+        <v>40</v>
+      </c>
+      <c r="E73" s="22">
+        <v>30</v>
+      </c>
+      <c r="K73" s="22">
+        <v>60</v>
+      </c>
+      <c r="L73" s="22">
+        <v>50</v>
+      </c>
+      <c r="M73" s="22">
+        <v>40</v>
+      </c>
+      <c r="N73" s="22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74" s="22">
+        <v>0</v>
+      </c>
+      <c r="B74" s="42">
+        <v>1.08526998481558E-4</v>
+      </c>
+      <c r="C74" s="42">
+        <v>1.0974513043231201E-4</v>
+      </c>
+      <c r="D74" s="42">
+        <v>1.12682126063935E-4</v>
+      </c>
+      <c r="E74" s="42">
+        <v>9.9277883230108007E-5</v>
+      </c>
+      <c r="G74" s="37"/>
+      <c r="J74" s="22">
+        <v>0</v>
+      </c>
+      <c r="K74" s="42">
+        <v>4.0065379109304601E-5</v>
+      </c>
+      <c r="L74" s="42">
+        <v>1.29839123484923E-4</v>
+      </c>
+      <c r="M74" s="42">
+        <v>3.96577796146004E-4</v>
+      </c>
+      <c r="N74" s="42">
+        <v>1.2625203199401001E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75" s="22">
+        <f t="shared" ref="A75:A80" si="12">A74+15</f>
+        <v>15</v>
+      </c>
+      <c r="B75" s="42">
+        <v>4.2097443873959501E-4</v>
+      </c>
+      <c r="C75" s="42">
+        <v>4.1716290738053898E-4</v>
+      </c>
+      <c r="D75" s="42">
+        <v>4.32318321801057E-4</v>
+      </c>
+      <c r="E75" s="42">
+        <v>3.8653389456714897E-4</v>
+      </c>
+      <c r="G75" s="37"/>
+      <c r="J75" s="22">
+        <f t="shared" ref="J75:J80" si="13">J74+15</f>
+        <v>15</v>
+      </c>
+      <c r="K75" s="42">
+        <v>4.1301850461261998E-5</v>
+      </c>
+      <c r="L75" s="42">
+        <v>1.27879864515799E-4</v>
+      </c>
+      <c r="M75" s="42">
+        <v>4.03234742498921E-4</v>
+      </c>
+      <c r="N75" s="42">
+        <v>1.26735408774957E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76" s="22">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="B76" s="42">
+        <v>1.20217753866611E-3</v>
+      </c>
+      <c r="C76" s="42">
+        <v>1.2026441252108E-3</v>
+      </c>
+      <c r="D76" s="42">
+        <v>1.21655599494351E-3</v>
+      </c>
+      <c r="E76" s="42">
+        <v>1.1377481996397501E-3</v>
+      </c>
+      <c r="G76" s="37"/>
+      <c r="J76" s="22">
+        <f t="shared" si="13"/>
+        <v>30</v>
+      </c>
+      <c r="K76" s="42">
+        <v>4.3128724138504603E-5</v>
+      </c>
+      <c r="L76" s="42">
+        <v>1.3423452245478999E-4</v>
+      </c>
+      <c r="M76" s="42">
+        <v>4.3606047762709998E-4</v>
+      </c>
+      <c r="N76" s="42">
+        <v>1.44592646278795E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77" s="22">
+        <f t="shared" si="12"/>
+        <v>45</v>
+      </c>
+      <c r="B77" s="42">
+        <v>2.4373485454174302E-3</v>
+      </c>
+      <c r="C77" s="42">
+        <v>2.4277435970044398E-3</v>
+      </c>
+      <c r="D77" s="42">
+        <v>2.4172958685149499E-3</v>
+      </c>
+      <c r="E77" s="42">
+        <v>2.3737118255027102E-3</v>
+      </c>
+      <c r="G77" s="37"/>
+      <c r="J77" s="22">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="K77" s="42">
+        <v>4.506147540637E-5</v>
+      </c>
+      <c r="L77" s="42">
+        <v>1.45445305501056E-4</v>
+      </c>
+      <c r="M77" s="42">
+        <v>4.7081346813079101E-4</v>
+      </c>
+      <c r="N77" s="42">
+        <v>1.4326410853651001E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A78" s="22">
+        <f t="shared" si="12"/>
+        <v>60</v>
+      </c>
+      <c r="B78" s="42">
+        <v>3.9263760522917903E-3</v>
+      </c>
+      <c r="C78" s="42">
+        <v>3.9282097005555001E-3</v>
+      </c>
+      <c r="D78" s="42">
+        <v>3.9138729275940698E-3</v>
+      </c>
+      <c r="E78" s="42">
+        <v>3.8422086938569499E-3</v>
+      </c>
+      <c r="G78" s="37"/>
+      <c r="J78" s="22">
+        <f t="shared" si="13"/>
+        <v>60</v>
+      </c>
+      <c r="K78" s="42">
+        <v>4.7969085630769702E-5</v>
+      </c>
+      <c r="L78" s="42">
+        <v>1.4714183496513099E-4</v>
+      </c>
+      <c r="M78" s="42">
+        <v>4.84844799503978E-4</v>
+      </c>
+      <c r="N78" s="42">
+        <v>1.53617133378922E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A79" s="22">
+        <f t="shared" si="12"/>
+        <v>75</v>
+      </c>
+      <c r="B79" s="42">
+        <v>5.1707163210417103E-3</v>
+      </c>
+      <c r="C79" s="42">
+        <v>5.1711454196450698E-3</v>
+      </c>
+      <c r="D79" s="42">
+        <v>5.1767069336665101E-3</v>
+      </c>
+      <c r="E79" s="42">
+        <v>5.2238834842917503E-3</v>
+      </c>
+      <c r="G79" s="37"/>
+      <c r="J79" s="22">
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+      <c r="K79" s="42">
+        <v>5.25054376108973E-5</v>
+      </c>
+      <c r="L79" s="42">
+        <v>1.6732389004285399E-4</v>
+      </c>
+      <c r="M79" s="42">
+        <v>5.0108971349993104E-4</v>
+      </c>
+      <c r="N79" s="42">
+        <v>1.62802610157884E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A80" s="22">
+        <f t="shared" si="12"/>
+        <v>90</v>
+      </c>
+      <c r="B80" s="42">
+        <v>5.5312892936176996E-3</v>
+      </c>
+      <c r="C80" s="42">
+        <v>5.53349753447908E-3</v>
+      </c>
+      <c r="D80" s="42">
+        <v>5.52443854796595E-3</v>
+      </c>
+      <c r="E80" s="42">
+        <v>5.5300708712140399E-3</v>
+      </c>
+      <c r="G80" s="37"/>
+      <c r="J80" s="22">
+        <f t="shared" si="13"/>
+        <v>90</v>
+      </c>
+      <c r="K80" s="42">
+        <v>5.27304000016645E-5</v>
+      </c>
+      <c r="L80" s="42">
+        <v>1.5756128707651801E-4</v>
+      </c>
+      <c r="M80" s="42">
+        <v>5.1780473377178104E-4</v>
+      </c>
+      <c r="N80" s="42">
+        <v>1.61252640875811E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>218</v>
+      </c>
+      <c r="C87" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>219</v>
+      </c>
+      <c r="C88">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>220</v>
+      </c>
+      <c r="C89" s="38">
+        <f>C88-C87*C88</f>
+        <v>59.999940000000002</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="C92" s="8"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C93" s="44">
+        <v>-2.9046972986323001E-5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C94" s="44">
+        <f>C93/60</f>
+        <v>-4.841162164387167E-7</v>
       </c>
     </row>
   </sheetData>
@@ -13229,60 +13624,60 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">

</xml_diff>

<commit_message>
just to sync, overwrite it please
</commit_message>
<xml_diff>
--- a/AMPS2019/EXTENDED/comparisons.xlsx
+++ b/AMPS2019/EXTENDED/comparisons.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779368AB-42CE-4752-8795-B9693917E139}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FE" sheetId="4" r:id="rId1"/>
     <sheet name="EPS comparison" sheetId="2" r:id="rId2"/>
     <sheet name="II-B2-FE" sheetId="1" r:id="rId3"/>
     <sheet name="EPS-case1" sheetId="6" r:id="rId4"/>
-    <sheet name="EPS-case3" sheetId="5" r:id="rId5"/>
+    <sheet name="EPS-case2" sheetId="7" r:id="rId5"/>
+    <sheet name="EPS-case3" sheetId="5" r:id="rId6"/>
+    <sheet name="guidelines" sheetId="8" r:id="rId7"/>
+    <sheet name="Planilha3" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="138">
   <si>
     <t>FE_std_HE</t>
   </si>
@@ -365,22 +369,98 @@
   <si>
     <t>CASO 1</t>
   </si>
+  <si>
+    <t>&gt;&gt; o desempenho é aparentemente insensível a variações em lambda theta entre 0.5 e 10</t>
+  </si>
+  <si>
+    <t>&gt;&gt; fixando lambda_theta em 2, o desempenho fica semelhante com lambda a entre 1.5 e 5</t>
+  </si>
+  <si>
+    <t>CASO 2</t>
+  </si>
+  <si>
+    <t>CASO2</t>
+  </si>
+  <si>
+    <t>OK, há alguma sensibilidade com lambda.</t>
+  </si>
+  <si>
+    <t>Mas antes disso, seguindo a linha do que o PE escreveu, precisamos:</t>
+  </si>
+  <si>
+    <t>retirar os operadores mediana desnecessários</t>
+  </si>
+  <si>
+    <t>a) performance sensibility wrt the choice of lambda, polynomial order d, and fixed threshold values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c) investigate the source of bias in the phasor frequency estimate and a way to compensate for it. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">b) to remove the arbitrary choices of the fixed threshold values, I would strongly recommend you to re-think the formulation of the detectors, 
+in order to remove the unnecessary median operators and to incorporate the maximum variation of the smooth function s[n] as a means to guide the threshold choice. </t>
+  </si>
+  <si>
+    <t>Estudo do detector de magnitude</t>
+  </si>
+  <si>
+    <t>1 - retiramos o operador mediana desnecessário</t>
+  </si>
+  <si>
+    <t>Não houve alteração no desempenho.</t>
+  </si>
+  <si>
+    <t>2 - investigar a variação normal do sinal de detecção e os valores típicos de pico.</t>
+  </si>
+  <si>
+    <t>3 - determinar um valor de limiar condizente com 2</t>
+  </si>
+  <si>
+    <t>Como?</t>
+  </si>
+  <si>
+    <t>Vamos começar pelo pior caso para magnitude</t>
+  </si>
+  <si>
+    <t>SNR = 30db</t>
+  </si>
+  <si>
+    <t>Ph = 90 graus</t>
+  </si>
+  <si>
+    <t>provavelmente há influência de lambda_a</t>
+  </si>
+  <si>
+    <t>Escolhemos d = 0, polinomio constante.</t>
+  </si>
+  <si>
+    <t>Para o caso 1, com SNR 60 db e phi0 = 90 graus</t>
+  </si>
+  <si>
+    <t>SNR = 30</t>
+  </si>
+  <si>
+    <t>Para fins de determinação do limiar, precisamos definir uma variação normal de dm.</t>
+  </si>
+  <si>
+    <t>para d = 1, entre os pontos 0 a 200</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="10">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
-    <numFmt numFmtId="172" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="173" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -521,28 +601,28 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -556,6 +636,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,7 +659,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -615,7 +698,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -724,7 +807,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3EEA-4B85-927C-A7AEAD4C23BC}"/>
             </c:ext>
@@ -796,7 +879,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="164084264"/>
@@ -858,7 +941,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="164084656"/>
@@ -899,7 +982,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -911,7 +994,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -950,7 +1033,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1059,7 +1142,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-559D-4750-AAF7-10F1CE6B8113}"/>
             </c:ext>
@@ -1131,7 +1214,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="239852432"/>
@@ -1193,7 +1276,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="239852824"/>
@@ -1234,7 +1317,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2377,7 +2460,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2413,7 +2496,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2434,10 +2517,259 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>387994</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{747B3E4E-4419-4A1F-8B09-019B09CABF09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6126480" y="883920"/>
+          <a:ext cx="4015114" cy="3009900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>319342</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB95F7B9-C91A-4BF2-8262-737B9B820276}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6210300" y="3893820"/>
+          <a:ext cx="3862642" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>461679</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12249CF8-CCD7-4C14-BFA7-4C1D1EF86AED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6149340" y="6774180"/>
+          <a:ext cx="4065939" cy="3048000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>67118</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB13BAD8-4652-46A2-9144-1B4D17953BDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9974580" y="6697979"/>
+          <a:ext cx="4084320" cy="3061779"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2475,7 +2807,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2510,6 +2842,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2545,9 +2894,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2720,41 +3086,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>44</v>
       </c>
@@ -2768,7 +3134,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>39</v>
       </c>
@@ -2800,7 +3166,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -2836,7 +3202,7 @@
         <v>4.6525502333783298E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -2872,7 +3238,7 @@
         <v>0.131483936121503</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>37</v>
       </c>
@@ -2886,7 +3252,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>39</v>
       </c>
@@ -2918,7 +3284,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -2954,7 +3320,7 @@
         <v>1.2548237159175499</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -2990,7 +3356,7 @@
         <v>0.26649080307221995</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>38</v>
       </c>
@@ -3004,7 +3370,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>39</v>
       </c>
@@ -3036,7 +3402,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>7</v>
       </c>
@@ -3072,7 +3438,7 @@
         <v>1.1684859453060001</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>8</v>
       </c>
@@ -3114,26 +3480,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:Z69"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="W5" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>61</v>
       </c>
@@ -3160,7 +3526,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -3192,7 +3558,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -3236,7 +3602,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -3279,7 +3645,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" ref="A10:A15" si="1">A9+15</f>
         <v>15</v>
@@ -3323,7 +3689,7 @@
         <v>39.200000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -3364,7 +3730,7 @@
         <v>48.5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -3408,7 +3774,7 @@
         <v>53.3</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -3452,7 +3818,7 @@
         <v>53.3</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -3480,7 +3846,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -3505,17 +3871,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="Q16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -3532,13 +3898,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
       <c r="E19" s="14"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" ref="A20:A25" si="2">A19+15</f>
         <v>15</v>
@@ -3551,7 +3917,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -3571,7 +3937,7 @@
       </c>
       <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -3584,7 +3950,7 @@
         <v>1.0699999999999999E-11</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="2"/>
         <v>60</v>
@@ -3597,14 +3963,14 @@
         <v>1.2400000000000001E-9</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="E24" s="14"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="2"/>
         <v>90</v>
@@ -3629,7 +3995,7 @@
         <v>1.7017543859649122</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -3641,7 +4007,7 @@
         <v>266355140.1869159</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -3665,7 +4031,7 @@
         <v>2298387.0967741935</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
@@ -3674,7 +4040,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" ref="A29:A34" si="3">A28+15</f>
         <v>15</v>
@@ -3687,7 +4053,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -3697,50 +4063,50 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="E31" s="14"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="E32" s="14"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
       <c r="E33" s="14"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
       <c r="E34" s="14"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -3760,7 +4126,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0</v>
       </c>
@@ -3780,7 +4146,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" ref="A42:A47" si="4">A41+15</f>
         <v>15</v>
@@ -3801,7 +4167,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="4"/>
         <v>30</v>
@@ -3822,7 +4188,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="4"/>
         <v>45</v>
@@ -3840,7 +4206,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="4"/>
         <v>60</v>
@@ -3858,7 +4224,7 @@
         <v>31.8</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="4"/>
         <v>75</v>
@@ -3879,7 +4245,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="4"/>
         <v>90</v>
@@ -3900,12 +4266,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -3922,7 +4288,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>0</v>
       </c>
@@ -3939,7 +4305,7 @@
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" ref="A53:A58" si="5">A52+15</f>
         <v>15</v>
@@ -3957,7 +4323,7 @@
         <v>27.1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="5"/>
         <v>30</v>
@@ -3975,7 +4341,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="5"/>
         <v>45</v>
@@ -3993,7 +4359,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="5"/>
         <v>60</v>
@@ -4011,7 +4377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="5"/>
         <v>75</v>
@@ -4029,7 +4395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="5"/>
         <v>90</v>
@@ -4047,12 +4413,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>50</v>
       </c>
@@ -4069,7 +4435,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>0</v>
       </c>
@@ -4086,7 +4452,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" ref="A64:A69" si="6">A63+15</f>
         <v>15</v>
@@ -4104,7 +4470,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="6"/>
         <v>30</v>
@@ -4122,7 +4488,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="6"/>
         <v>45</v>
@@ -4140,7 +4506,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" si="6"/>
         <v>60</v>
@@ -4158,7 +4524,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <f t="shared" si="6"/>
         <v>75</v>
@@ -4176,7 +4542,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="6"/>
         <v>90</v>
@@ -4200,46 +4566,46 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E14" sqref="E14:H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -4259,7 +4625,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4279,17 +4645,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -4318,7 +4684,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -4347,7 +4713,7 @@
         <v>3.2802614457142702E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -4376,7 +4742,7 @@
         <v>4.5071145312710101E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -4393,7 +4759,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -4431,7 +4797,7 @@
         <v>2.0769202567494901E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -4469,12 +4835,12 @@
         <v>4.4871321568041602E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -4503,7 +4869,7 @@
         <v>9.2702022162879298E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -4532,18 +4898,18 @@
         <v>4.9477639907994698E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -4572,7 +4938,7 @@
         <v>1.0209234467157E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -4601,29 +4967,29 @@
         <v>8.9328868849508105E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G30" s="6"/>
       <c r="J30" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -4632,7 +4998,7 @@
         <v>2.1605377722768151E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -4653,24 +5019,24 @@
         <v>-6.9987981883495171E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -4687,7 +5053,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -4704,7 +5070,7 @@
         <v>-1.8357987678080999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B40" s="1">
         <v>1.3870852577291001E-5</v>
       </c>
@@ -4718,7 +5084,7 @@
         <v>4.3177118710681502E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -4738,7 +5104,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B43" s="1">
         <v>1.632029604517E-5</v>
       </c>
@@ -4755,12 +5121,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="G44" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -4780,7 +5146,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B46" s="1">
         <v>1.7113734935356899E-5</v>
       </c>
@@ -4806,7 +5172,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H47">
         <v>10</v>
       </c>
@@ -4820,7 +5186,7 @@
         <v>1.4458157246083101E-5</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -4850,7 +5216,7 @@
         <v>1.8148094370953901E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B49" s="1">
         <v>1.73263306517101E-5</v>
       </c>
@@ -4877,7 +5243,7 @@
         <v>3.5223250677112199E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H50">
         <f t="shared" ref="H50:H55" si="1">H49+15</f>
         <v>45</v>
@@ -4892,7 +5258,7 @@
         <v>4.9611771021625703E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>28</v>
       </c>
@@ -4922,7 +5288,7 @@
         <v>5.0677305705378397E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B52" s="1">
         <v>2.0277905166956101E-5</v>
       </c>
@@ -4949,7 +5315,7 @@
         <v>5.7550877009226596E-4</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H53">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -4964,7 +5330,7 @@
         <v>5.53791658750513E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -4994,7 +5360,7 @@
         <v>5.97704462378584E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B55" s="1">
         <v>1.9175126747274499E-5</v>
       </c>
@@ -5028,16 +5394,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A12:AU76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A4:AU76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K8" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15:W21"/>
+    <sheetView topLeftCell="K28" workbookViewId="0">
+      <selection activeCell="S34" sqref="S34:W43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="12" spans="19:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="19:35" x14ac:dyDescent="0.3">
+      <c r="S4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="19:35" x14ac:dyDescent="0.3">
+      <c r="S5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="19:35" x14ac:dyDescent="0.3">
       <c r="U12" t="s">
         <v>88</v>
       </c>
@@ -5069,7 +5445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="19:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S13" s="17" t="s">
         <v>112</v>
       </c>
@@ -5107,7 +5483,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="19:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S14" t="s">
         <v>50</v>
       </c>
@@ -5154,7 +5530,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="19:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S15">
         <v>0</v>
       </c>
@@ -5201,7 +5577,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="16" spans="19:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S16">
         <f t="shared" ref="S16:S21" si="0">S15+15</f>
         <v>15</v>
@@ -5251,7 +5627,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
       <c r="S17">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -5301,7 +5677,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="S18">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -5351,7 +5727,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="S19">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -5401,7 +5777,7 @@
         <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="S20">
         <f t="shared" si="0"/>
         <v>75</v>
@@ -5451,7 +5827,7 @@
         <v>62.8</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="S21">
         <f t="shared" si="0"/>
         <v>90</v>
@@ -5501,7 +5877,7 @@
         <v>86.6</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -5536,7 +5912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>112</v>
       </c>
@@ -5586,7 +5962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -5648,7 +6024,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
@@ -5710,7 +6086,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" ref="A27:A32" si="3">A26+15</f>
         <v>15</v>
@@ -5776,7 +6152,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -5842,7 +6218,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="3"/>
         <v>45</v>
@@ -5908,7 +6284,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="3"/>
         <v>60</v>
@@ -5974,7 +6350,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="3"/>
         <v>75</v>
@@ -6040,7 +6416,7 @@
         <v>27.1</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="3"/>
         <v>90</v>
@@ -6106,8 +6482,8 @@
         <v>52.8</v>
       </c>
     </row>
-    <row r="33" spans="13:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="13:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="13:47" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="13:47" x14ac:dyDescent="0.3">
       <c r="O34" t="s">
         <v>88</v>
       </c>
@@ -6161,7 +6537,7 @@
       </c>
       <c r="AU34" s="22"/>
     </row>
-    <row r="35" spans="13:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="13:47" x14ac:dyDescent="0.3">
       <c r="M35" s="17" t="s">
         <v>112</v>
       </c>
@@ -6241,7 +6617,7 @@
       </c>
       <c r="AU35" s="22"/>
     </row>
-    <row r="36" spans="13:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="13:47" x14ac:dyDescent="0.3">
       <c r="M36" t="s">
         <v>50</v>
       </c>
@@ -6334,7 +6710,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="13:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="13:47" x14ac:dyDescent="0.3">
       <c r="M37">
         <v>0</v>
       </c>
@@ -6427,7 +6803,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="38" spans="13:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="13:47" x14ac:dyDescent="0.3">
       <c r="M38">
         <f t="shared" ref="M38:M43" si="7">M37+15</f>
         <v>15</v>
@@ -6526,7 +6902,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="39" spans="13:47" x14ac:dyDescent="0.25">
+    <row r="39" spans="13:47" x14ac:dyDescent="0.3">
       <c r="M39">
         <f t="shared" si="7"/>
         <v>30</v>
@@ -6625,7 +7001,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="40" spans="13:47" x14ac:dyDescent="0.25">
+    <row r="40" spans="13:47" x14ac:dyDescent="0.3">
       <c r="M40">
         <f t="shared" si="7"/>
         <v>45</v>
@@ -6724,7 +7100,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="41" spans="13:47" x14ac:dyDescent="0.25">
+    <row r="41" spans="13:47" x14ac:dyDescent="0.3">
       <c r="M41">
         <f t="shared" si="7"/>
         <v>60</v>
@@ -6823,7 +7199,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="42" spans="13:47" x14ac:dyDescent="0.25">
+    <row r="42" spans="13:47" x14ac:dyDescent="0.3">
       <c r="M42">
         <f t="shared" si="7"/>
         <v>75</v>
@@ -6922,7 +7298,7 @@
         <v>31.6</v>
       </c>
     </row>
-    <row r="43" spans="13:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="13:47" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M43">
         <f t="shared" si="7"/>
         <v>90</v>
@@ -7021,7 +7397,7 @@
         <v>61.5</v>
       </c>
     </row>
-    <row r="45" spans="13:47" x14ac:dyDescent="0.25">
+    <row r="45" spans="13:47" x14ac:dyDescent="0.3">
       <c r="S45" s="22"/>
       <c r="T45" s="22"/>
       <c r="U45" s="22" t="s">
@@ -7032,7 +7408,7 @@
       </c>
       <c r="W45" s="22"/>
     </row>
-    <row r="46" spans="13:47" x14ac:dyDescent="0.25">
+    <row r="46" spans="13:47" x14ac:dyDescent="0.3">
       <c r="S46" s="28" t="s">
         <v>112</v>
       </c>
@@ -7047,7 +7423,7 @@
       </c>
       <c r="W46" s="22"/>
     </row>
-    <row r="47" spans="13:47" x14ac:dyDescent="0.25">
+    <row r="47" spans="13:47" x14ac:dyDescent="0.3">
       <c r="S47" s="22" t="s">
         <v>50</v>
       </c>
@@ -7064,7 +7440,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="13:47" x14ac:dyDescent="0.25">
+    <row r="48" spans="13:47" x14ac:dyDescent="0.3">
       <c r="S48" s="22">
         <v>0</v>
       </c>
@@ -7081,7 +7457,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="49" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S49" s="22">
         <f t="shared" ref="S49:S54" si="13">S48+15</f>
         <v>15</v>
@@ -7099,7 +7475,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="50" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S50" s="22">
         <f t="shared" si="13"/>
         <v>30</v>
@@ -7117,7 +7493,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="51" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S51" s="22">
         <f t="shared" si="13"/>
         <v>45</v>
@@ -7135,7 +7511,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="52" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S52" s="22">
         <f t="shared" si="13"/>
         <v>60</v>
@@ -7153,7 +7529,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="53" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S53" s="22">
         <f t="shared" si="13"/>
         <v>75</v>
@@ -7171,7 +7547,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="54" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S54" s="22">
         <f t="shared" si="13"/>
         <v>90</v>
@@ -7189,7 +7565,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="56" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S56" s="22"/>
       <c r="T56" s="22"/>
       <c r="U56" s="22" t="s">
@@ -7200,7 +7576,7 @@
       </c>
       <c r="W56" s="22"/>
     </row>
-    <row r="57" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S57" s="28" t="s">
         <v>112</v>
       </c>
@@ -7215,7 +7591,7 @@
       </c>
       <c r="W57" s="22"/>
     </row>
-    <row r="58" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S58" s="22" t="s">
         <v>50</v>
       </c>
@@ -7232,7 +7608,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S59" s="22">
         <v>0</v>
       </c>
@@ -7249,7 +7625,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="60" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S60" s="22">
         <f t="shared" ref="S60:S65" si="14">S59+15</f>
         <v>15</v>
@@ -7267,7 +7643,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="61" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S61" s="22">
         <f t="shared" si="14"/>
         <v>30</v>
@@ -7285,7 +7661,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="62" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S62" s="22">
         <f t="shared" si="14"/>
         <v>45</v>
@@ -7303,7 +7679,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="63" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S63" s="22">
         <f t="shared" si="14"/>
         <v>60</v>
@@ -7321,7 +7697,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="64" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S64" s="22">
         <f t="shared" si="14"/>
         <v>75</v>
@@ -7339,7 +7715,7 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="65" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S65" s="22">
         <f t="shared" si="14"/>
         <v>90</v>
@@ -7357,7 +7733,7 @@
         <v>51.3</v>
       </c>
     </row>
-    <row r="67" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S67" s="22"/>
       <c r="T67" s="22"/>
       <c r="U67" s="22" t="s">
@@ -7368,7 +7744,7 @@
       </c>
       <c r="W67" s="22"/>
     </row>
-    <row r="68" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S68" s="28" t="s">
         <v>112</v>
       </c>
@@ -7383,7 +7759,7 @@
       </c>
       <c r="W68" s="22"/>
     </row>
-    <row r="69" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S69" s="22" t="s">
         <v>50</v>
       </c>
@@ -7400,7 +7776,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S70" s="22">
         <v>0</v>
       </c>
@@ -7417,7 +7793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S71" s="22">
         <f t="shared" ref="S71:S76" si="15">S70+15</f>
         <v>15</v>
@@ -7435,7 +7811,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="72" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S72" s="22">
         <f t="shared" si="15"/>
         <v>30</v>
@@ -7453,7 +7829,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="73" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S73" s="22">
         <f t="shared" si="15"/>
         <v>45</v>
@@ -7471,7 +7847,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="74" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S74" s="22">
         <f t="shared" si="15"/>
         <v>60</v>
@@ -7489,7 +7865,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="75" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S75" s="22">
         <f t="shared" si="15"/>
         <v>75</v>
@@ -7507,7 +7883,7 @@
         <v>28.8</v>
       </c>
     </row>
-    <row r="76" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="19:23" x14ac:dyDescent="0.3">
       <c r="S76" s="22">
         <f t="shared" si="15"/>
         <v>90</v>
@@ -8259,22 +8635,823 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF74377-79DE-4849-BD1C-400F46B034BE}">
+  <dimension ref="C12:M33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="12" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="19">
+        <v>1</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="L13" s="19">
+        <v>2</v>
+      </c>
+      <c r="M13" s="20"/>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C14" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="I14" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="K14" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="L14" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="M14" s="23"/>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C15" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="22">
+        <v>60</v>
+      </c>
+      <c r="E15" s="22">
+        <v>50</v>
+      </c>
+      <c r="F15" s="22">
+        <v>40</v>
+      </c>
+      <c r="G15" s="23">
+        <v>30</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="22">
+        <v>60</v>
+      </c>
+      <c r="K15" s="22">
+        <v>50</v>
+      </c>
+      <c r="L15" s="22">
+        <v>40</v>
+      </c>
+      <c r="M15" s="23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C16" s="24">
+        <v>0</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
+      <c r="I16" s="24">
+        <v>0</v>
+      </c>
+      <c r="J16" s="22">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="K16" s="22">
+        <v>59.3</v>
+      </c>
+      <c r="L16" s="22">
+        <v>55.1</v>
+      </c>
+      <c r="M16" s="23">
+        <v>58.4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C17" s="24">
+        <f t="shared" ref="C17:C22" si="0">C16+15</f>
+        <v>15</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23"/>
+      <c r="I17" s="24">
+        <f t="shared" ref="I17:I22" si="1">I16+15</f>
+        <v>15</v>
+      </c>
+      <c r="J17" s="22">
+        <v>100</v>
+      </c>
+      <c r="K17" s="22">
+        <v>99.9</v>
+      </c>
+      <c r="L17" s="22">
+        <v>89.9</v>
+      </c>
+      <c r="M17" s="23">
+        <v>81.5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C18" s="24">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="23"/>
+      <c r="I18" s="24">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="J18" s="22">
+        <v>100</v>
+      </c>
+      <c r="K18" s="22">
+        <v>99.9</v>
+      </c>
+      <c r="L18" s="22">
+        <v>85.1</v>
+      </c>
+      <c r="M18" s="23">
+        <v>70.3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C19" s="24">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23"/>
+      <c r="I19" s="24">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="J19" s="22">
+        <v>0</v>
+      </c>
+      <c r="K19" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="L19" s="22">
+        <v>20.7</v>
+      </c>
+      <c r="M19" s="23">
+        <v>40.9</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C20" s="24">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23"/>
+      <c r="I20" s="24">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="J20" s="22">
+        <v>0</v>
+      </c>
+      <c r="K20" s="22">
+        <v>0</v>
+      </c>
+      <c r="L20" s="22">
+        <v>0</v>
+      </c>
+      <c r="M20" s="23">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C21" s="24">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
+      <c r="I21" s="24">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="J21" s="22">
+        <v>0</v>
+      </c>
+      <c r="K21" s="22">
+        <v>0</v>
+      </c>
+      <c r="L21" s="22">
+        <v>0</v>
+      </c>
+      <c r="M21" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="25">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="27"/>
+      <c r="I22" s="25">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="J22" s="26">
+        <v>0</v>
+      </c>
+      <c r="K22" s="26">
+        <v>0</v>
+      </c>
+      <c r="L22" s="26">
+        <v>0</v>
+      </c>
+      <c r="M22" s="27">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C24" s="18"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="19">
+        <v>1</v>
+      </c>
+      <c r="G24" s="20"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="L24" s="19">
+        <v>2</v>
+      </c>
+      <c r="M24" s="20"/>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C25" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="22">
+        <v>2.5</v>
+      </c>
+      <c r="G25" s="23"/>
+      <c r="I25" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="J25" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="K25" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="L25" s="22">
+        <v>2.5</v>
+      </c>
+      <c r="M25" s="23"/>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C26" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="22">
+        <v>60</v>
+      </c>
+      <c r="E26" s="22">
+        <v>50</v>
+      </c>
+      <c r="F26" s="22">
+        <v>40</v>
+      </c>
+      <c r="G26" s="23">
+        <v>30</v>
+      </c>
+      <c r="I26" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="22">
+        <v>60</v>
+      </c>
+      <c r="K26" s="22">
+        <v>50</v>
+      </c>
+      <c r="L26" s="22">
+        <v>40</v>
+      </c>
+      <c r="M26" s="23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C27" s="24">
+        <v>0</v>
+      </c>
+      <c r="D27" s="22">
+        <v>83.5</v>
+      </c>
+      <c r="E27" s="22">
+        <v>63.8</v>
+      </c>
+      <c r="F27" s="22">
+        <v>56.5</v>
+      </c>
+      <c r="G27" s="23">
+        <v>58.6</v>
+      </c>
+      <c r="I27" s="24">
+        <v>0</v>
+      </c>
+      <c r="J27" s="22">
+        <v>83.7</v>
+      </c>
+      <c r="K27" s="22">
+        <v>58.2</v>
+      </c>
+      <c r="L27" s="22">
+        <v>56.8</v>
+      </c>
+      <c r="M27" s="23">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C28" s="24">
+        <f t="shared" ref="C28:C33" si="2">C27+15</f>
+        <v>15</v>
+      </c>
+      <c r="D28" s="22">
+        <v>100</v>
+      </c>
+      <c r="E28" s="22">
+        <v>100</v>
+      </c>
+      <c r="F28" s="22">
+        <v>97.7</v>
+      </c>
+      <c r="G28" s="23">
+        <v>83.1</v>
+      </c>
+      <c r="I28" s="24">
+        <f t="shared" ref="I28:I33" si="3">I27+15</f>
+        <v>15</v>
+      </c>
+      <c r="J28" s="22">
+        <v>100</v>
+      </c>
+      <c r="K28" s="22">
+        <v>100</v>
+      </c>
+      <c r="L28" s="22">
+        <v>97.9</v>
+      </c>
+      <c r="M28" s="23">
+        <v>84.3</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C29" s="24">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="D29" s="22">
+        <v>100</v>
+      </c>
+      <c r="E29" s="22">
+        <v>100</v>
+      </c>
+      <c r="F29" s="22">
+        <v>96.1</v>
+      </c>
+      <c r="G29" s="23">
+        <v>79.2</v>
+      </c>
+      <c r="I29" s="24">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="J29" s="22">
+        <v>100</v>
+      </c>
+      <c r="K29" s="22">
+        <v>100</v>
+      </c>
+      <c r="L29" s="22">
+        <v>96.6</v>
+      </c>
+      <c r="M29" s="23">
+        <v>79.3</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C30" s="24">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="D30" s="22">
+        <v>0</v>
+      </c>
+      <c r="E30" s="22">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F30" s="22">
+        <v>40.5</v>
+      </c>
+      <c r="G30" s="23">
+        <v>49.3</v>
+      </c>
+      <c r="I30" s="24">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="J30" s="22">
+        <v>0</v>
+      </c>
+      <c r="K30" s="22">
+        <v>18.5</v>
+      </c>
+      <c r="L30" s="22">
+        <v>41.5</v>
+      </c>
+      <c r="M30" s="23">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C31" s="24">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="D31" s="22">
+        <v>0</v>
+      </c>
+      <c r="E31" s="22">
+        <v>0</v>
+      </c>
+      <c r="F31" s="22">
+        <v>0</v>
+      </c>
+      <c r="G31" s="23">
+        <v>12.1</v>
+      </c>
+      <c r="I31" s="24">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="J31" s="22">
+        <v>0</v>
+      </c>
+      <c r="K31" s="22">
+        <v>0</v>
+      </c>
+      <c r="L31" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="M31" s="23">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C32" s="24">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="D32" s="22">
+        <v>0</v>
+      </c>
+      <c r="E32" s="22">
+        <v>0</v>
+      </c>
+      <c r="F32" s="22">
+        <v>0</v>
+      </c>
+      <c r="G32" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="I32" s="24">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="J32" s="22">
+        <v>0</v>
+      </c>
+      <c r="K32" s="22">
+        <v>0</v>
+      </c>
+      <c r="L32" s="22">
+        <v>0</v>
+      </c>
+      <c r="M32" s="23">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="25">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="D33" s="26">
+        <v>0</v>
+      </c>
+      <c r="E33" s="26">
+        <v>0</v>
+      </c>
+      <c r="F33" s="26">
+        <v>0</v>
+      </c>
+      <c r="G33" s="27">
+        <v>0</v>
+      </c>
+      <c r="I33" s="25">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="J33" s="26">
+        <v>0</v>
+      </c>
+      <c r="K33" s="26">
+        <v>0</v>
+      </c>
+      <c r="L33" s="26">
+        <v>0</v>
+      </c>
+      <c r="M33" s="27">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="L13">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="4.55"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16:M22">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="4.55"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L24">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="4.55"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J27:M33">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="4.55"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="4.55"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:G33">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="4.55"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="4.55"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:G22">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="4.55"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="4.55"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BG87"/>
   <sheetViews>
     <sheetView topLeftCell="AN52" workbookViewId="0">
       <selection activeCell="BD71" sqref="BD71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
-    <col min="13" max="13" width="3.28515625" style="16" customWidth="1"/>
-    <col min="28" max="28" width="8.85546875" style="17"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="13" max="13" width="3.33203125" style="16" customWidth="1"/>
+    <col min="28" max="28" width="8.88671875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>103</v>
       </c>
@@ -8282,12 +9459,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="V2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -8307,12 +9484,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -8329,7 +9506,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -8340,12 +9517,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -8383,7 +9560,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -8430,7 +9607,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
@@ -8465,7 +9642,7 @@
         <v>46.1</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" ref="A11:A16" si="0">A10+15</f>
         <v>15</v>
@@ -8503,7 +9680,7 @@
         <v>38.6</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -8541,7 +9718,7 @@
         <v>57.2</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -8579,7 +9756,7 @@
         <v>54.1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -8617,7 +9794,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>75</v>
@@ -8655,7 +9832,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>90</v>
@@ -8693,7 +9870,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -8731,7 +9908,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -8778,7 +9955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -8813,7 +9990,7 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" ref="A21:A26" si="3">A20+15</f>
         <v>15</v>
@@ -8851,7 +10028,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -8889,7 +10066,7 @@
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="3"/>
         <v>45</v>
@@ -8927,7 +10104,7 @@
         <v>43.1</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="3"/>
         <v>60</v>
@@ -8965,7 +10142,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="3"/>
         <v>75</v>
@@ -9003,7 +10180,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="3"/>
         <v>90</v>
@@ -9047,7 +10224,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AE27" s="17" t="s">
         <v>109</v>
       </c>
@@ -9061,7 +10238,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="P28" s="8" t="s">
         <v>102</v>
       </c>
@@ -9081,7 +10258,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -9134,7 +10311,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -9197,7 +10374,7 @@
         <v>22.6</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -9260,7 +10437,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" ref="A32:A37" si="7">A31+15</f>
         <v>15</v>
@@ -9326,7 +10503,7 @@
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="7"/>
         <v>30</v>
@@ -9392,7 +10569,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="34" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="7"/>
         <v>45</v>
@@ -9458,7 +10635,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="35" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="7"/>
         <v>60</v>
@@ -9524,7 +10701,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="7"/>
         <v>75</v>
@@ -9574,7 +10751,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="7"/>
         <v>90</v>
@@ -9642,7 +10819,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:51" x14ac:dyDescent="0.3">
       <c r="I38" t="s">
         <v>107</v>
       </c>
@@ -9683,7 +10860,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -9778,7 +10955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -9885,7 +11062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0</v>
       </c>
@@ -9983,7 +11160,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" ref="A42:A47" si="13">A41+15</f>
         <v>15</v>
@@ -10085,7 +11262,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="43" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="13"/>
         <v>30</v>
@@ -10187,7 +11364,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="44" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="13"/>
         <v>45</v>
@@ -10289,7 +11466,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="45" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="13"/>
         <v>60</v>
@@ -10391,7 +11568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="13"/>
         <v>75</v>
@@ -10493,7 +11670,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="13"/>
         <v>90</v>
@@ -10547,7 +11724,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:51" x14ac:dyDescent="0.3">
       <c r="AG48" t="s">
         <v>88</v>
       </c>
@@ -10567,7 +11744,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -10665,7 +11842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -10787,7 +11964,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>0</v>
       </c>
@@ -10897,7 +12074,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="52" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" ref="A52:A57" si="17">A51+15</f>
         <v>15</v>
@@ -11015,7 +12192,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="53" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="17"/>
         <v>30</v>
@@ -11133,7 +12310,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="54" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="17"/>
         <v>45</v>
@@ -11251,7 +12428,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="55" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="17"/>
         <v>60</v>
@@ -11369,7 +12546,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="56" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="17"/>
         <v>75</v>
@@ -11487,7 +12664,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="57" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="17"/>
         <v>90</v>
@@ -11605,8 +12782,8 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="58" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:59" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="59" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -11653,7 +12830,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="60" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>50</v>
       </c>
@@ -11722,7 +12899,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="61" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>0</v>
       </c>
@@ -11799,7 +12976,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" ref="A62:A67" si="25">A61+15</f>
         <v>15</v>
@@ -11878,7 +13055,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="63" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="25"/>
         <v>30</v>
@@ -11960,7 +13137,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="64" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="25"/>
         <v>45</v>
@@ -12042,7 +13219,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="65" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="25"/>
         <v>60</v>
@@ -12124,7 +13301,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="66" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="25"/>
         <v>75</v>
@@ -12206,7 +13383,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="67" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" si="25"/>
         <v>90</v>
@@ -12288,7 +13465,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="68" spans="1:59" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:59" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AQ68">
         <f t="shared" si="27"/>
         <v>90</v>
@@ -12338,7 +13515,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="69" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -12352,7 +13529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>50</v>
       </c>
@@ -12375,7 +13552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>0</v>
       </c>
@@ -12404,7 +13581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" ref="A72:A77" si="30">A71+15</f>
         <v>15</v>
@@ -12437,7 +13614,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="30"/>
         <v>30</v>
@@ -12470,7 +13647,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="30"/>
         <v>45</v>
@@ -12504,7 +13681,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="75" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A75">
         <f t="shared" si="30"/>
         <v>60</v>
@@ -12538,7 +13715,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="76" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="30"/>
         <v>75</v>
@@ -12572,7 +13749,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="77" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="30"/>
         <v>90</v>
@@ -12606,7 +13783,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="78" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:59" x14ac:dyDescent="0.3">
       <c r="AW78">
         <f t="shared" si="31"/>
         <v>75</v>
@@ -12624,7 +13801,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>48</v>
       </c>
@@ -12654,7 +13831,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>50</v>
       </c>
@@ -12671,7 +13848,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>0</v>
       </c>
@@ -12691,7 +13868,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <f t="shared" ref="A82:A87" si="32">A81+15</f>
         <v>15</v>
@@ -12709,7 +13886,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="32"/>
         <v>30</v>
@@ -12727,7 +13904,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="32"/>
         <v>45</v>
@@ -12745,7 +13922,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="32"/>
         <v>60</v>
@@ -12763,7 +13940,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="32"/>
         <v>75</v>
@@ -12781,7 +13958,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <f t="shared" si="32"/>
         <v>90</v>
@@ -13739,4 +14916,138 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A5B593-7303-4FD6-9DD3-49C9E2A199A3}">
+  <dimension ref="B2:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="106.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA0B435-11BA-4F6B-828D-D8267F154868}">
+  <dimension ref="B2:R16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>134</v>
+      </c>
+      <c r="R3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="K4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="R6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>128</v>
+      </c>
+      <c r="R8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>